<commit_message>
add measurement and adjust drawing of hex bolt
</commit_message>
<xml_diff>
--- a/Measurements/024 VISE SCREW extension/419GC31M.xlsx
+++ b/Measurements/024 VISE SCREW extension/419GC31M.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e5a9c027fd1ff47/Desktop/Meng/solidworks/Measurements/024 VISE SCREW extension/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoe\Meng\solidworks\Measurements\024 VISE SCREW extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{36B1F4D3-D5E2-47AB-8189-FDD1FD54DDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4577CACF-E731-4C89-94BB-1C18E15283F3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3834276-DB3A-4D44-9D25-FF4DF55082BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E6338A5-4ADC-4920-82B5-73ABC98241B7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>8.81</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Sample Measurement Record</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
@@ -525,10 +528,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,8 +619,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="0" y="2452116"/>
-          <a:ext cx="6607397" cy="3845568"/>
+          <a:off x="0" y="2381250"/>
+          <a:ext cx="6144482" cy="3696216"/>
           <a:chOff x="0" y="2381250"/>
           <a:chExt cx="6144482" cy="3696216"/>
         </a:xfrm>
@@ -1864,6 +1867,68 @@
               </a:solidFill>
             </a:rPr>
             <a:t>I</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="261546" cy="374077"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="TextBox 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{852B769C-CD33-400E-B5DD-5193DCA4DB17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2505075" y="2905125"/>
+          <a:ext cx="261546" cy="374077"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>J</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2193,7 +2258,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="A1:M22"/>
+      <selection activeCell="R16" sqref="R15:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
@@ -2205,21 +2270,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:16" ht="26.45" customHeight="1" thickBot="1">
       <c r="A2" s="26" t="s">
@@ -2271,7 +2336,9 @@
       <c r="J3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="19"/>
+      <c r="K3" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="L3" s="19"/>
       <c r="M3" s="18"/>
       <c r="P3" s="17"/>
@@ -2308,7 +2375,10 @@
       <c r="J4" s="15">
         <v>2.99</v>
       </c>
-      <c r="K4" s="15"/>
+      <c r="K4" s="15">
+        <f>1.85/2</f>
+        <v>0.92500000000000004</v>
+      </c>
       <c r="L4" s="15"/>
       <c r="M4" s="14"/>
     </row>
@@ -2344,7 +2414,10 @@
       <c r="J5" s="11">
         <v>2.97</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="11">
+        <f>1.686/2</f>
+        <v>0.84299999999999997</v>
+      </c>
       <c r="L5" s="11"/>
       <c r="M5" s="10"/>
     </row>
@@ -2380,7 +2453,10 @@
       <c r="J6" s="11">
         <v>2.97</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="11">
+        <f>1.924/2</f>
+        <v>0.96199999999999997</v>
+      </c>
       <c r="L6" s="11"/>
       <c r="M6" s="10"/>
     </row>
@@ -2416,7 +2492,10 @@
       <c r="J7" s="11">
         <v>2.99</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="K7" s="11">
+        <f>1.613/2</f>
+        <v>0.80649999999999999</v>
+      </c>
       <c r="L7" s="11"/>
       <c r="M7" s="10"/>
     </row>
@@ -2430,7 +2509,7 @@
       <c r="C8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <f>C8-E8</f>
         <v>0.67999999999999972</v>
       </c>
@@ -2452,7 +2531,10 @@
       <c r="J8" s="6">
         <v>2.98</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="6">
+        <f>1.728/2</f>
+        <v>0.86399999999999999</v>
+      </c>
       <c r="L8" s="6"/>
       <c r="M8" s="5"/>
     </row>

</xml_diff>